<commit_message>
Clean-up, error fixes with duplicate statements in compiled CSS, and started layout design.
</commit_message>
<xml_diff>
--- a/misc/notes.xlsx
+++ b/misc/notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\finap\git\cs480\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\finap\git\cs480\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,12 +39,6 @@
     <t>HTML</t>
   </si>
   <si>
-    <t>CSS</t>
-  </si>
-  <si>
-    <t>JavaScript</t>
-  </si>
-  <si>
     <t>PHP</t>
   </si>
   <si>
@@ -182,9 +177,6 @@
     <t>date/time</t>
   </si>
   <si>
-    <t>Users can comment on shared tasks</t>
-  </si>
-  <si>
     <t>Quick add</t>
   </si>
   <si>
@@ -209,10 +201,19 @@
     <t>F</t>
   </si>
   <si>
-    <t>&lt; 67</t>
-  </si>
-  <si>
     <t>Responsive</t>
+  </si>
+  <si>
+    <t>&lt; 64</t>
+  </si>
+  <si>
+    <t>CSS (SASS)</t>
+  </si>
+  <si>
+    <t>JavaScript + jQuery</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;= 94</t>
   </si>
 </sst>
 </file>
@@ -256,10 +257,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J47"/>
+  <dimension ref="B2:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +568,7 @@
       </c>
       <c r="C2" s="1">
         <f>SUM(C3:C6)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -569,7 +576,7 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -580,54 +587,54 @@
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
         <f>SUM(C9:C12)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -638,64 +645,64 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" t="s">
         <v>48</v>
-      </c>
-      <c r="I11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1">
         <f>SUM(C15:C17)</f>
@@ -704,53 +711,53 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="G15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="E16">
-        <v>101</v>
-      </c>
-      <c r="F16">
-        <v>89</v>
-      </c>
-      <c r="G16">
-        <v>78</v>
-      </c>
-      <c r="H16">
-        <v>67</v>
-      </c>
-      <c r="I16" t="s">
-        <v>61</v>
+      <c r="E16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="3">
+        <v>84</v>
+      </c>
+      <c r="G16" s="3">
+        <v>74</v>
+      </c>
+      <c r="H16" s="3">
+        <v>64</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -758,7 +765,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1">
         <f>SUM(C20:C27)</f>
@@ -767,7 +774,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2">
         <v>5</v>
@@ -775,7 +782,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -783,7 +790,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -791,7 +798,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -799,7 +806,7 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -807,7 +814,7 @@
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -815,7 +822,7 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -823,7 +830,7 @@
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -831,16 +838,16 @@
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1">
         <f>SUM(C30:C34)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C30" s="2">
         <v>5</v>
@@ -848,7 +855,7 @@
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -856,7 +863,7 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -864,7 +871,7 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -872,24 +879,24 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C36" s="1">
-        <f>SUM(C37:C39)</f>
-        <v>14</v>
+        <f>SUM(C37:C38)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -897,68 +904,60 @@
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="1">
+        <f>SUM(C41:C44)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41">
         <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="1">
-        <f>SUM(C42:C45)</f>
-        <v>15</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C47" s="1">
-        <f>C41+C36+C29+C19+C8+C14+C2</f>
-        <v>108</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="1">
+        <f>C40+C36+C29+C19+C8+C14+C2</f>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>